<commit_message>
+ Big fix and change + Integrate generating keyword into data analyzing + Delete processed file if it doesn't correspond to original data
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED22BD18-6528-4750-AF33-7C0A28D0143E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30FEC72-617D-4EE8-9459-F1356EE83E9A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="error" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>read stopwords_file bug charmap</t>
   </si>
@@ -142,9 +142,6 @@
     <t>sign</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>amcharts</t>
+  </si>
+  <si>
+    <t>PaperToKeyword</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -434,6 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,10 +765,10 @@
         <v>43105</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -780,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3704EA6-8F9B-4FB1-B218-0136F76D7AB7}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -881,7 +882,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -891,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -900,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -909,25 +910,34 @@
         <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11">
+        <v>4</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="10"/>
     </row>
@@ -941,7 +951,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -953,16 +963,16 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1005,15 +1015,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1023,7 +1033,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401364AE-1BC6-424E-9E40-562D0F35A9F2}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1056,10 +1066,10 @@
         <v>20</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5">
@@ -1067,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4">
         <v>3.6</v>
@@ -1079,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1089,10 +1099,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -1101,10 +1111,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -1113,10 +1123,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -1125,13 +1135,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5">
@@ -1139,13 +1149,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5">
@@ -1153,13 +1163,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5">
@@ -1167,7 +1177,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1206,69 +1216,69 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>